<commit_message>
Taux mensuel avec CA mensuel ok
</commit_message>
<xml_diff>
--- a/dataFormatts.xlsx
+++ b/dataFormatts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stage\AllWebScraping_VirtualGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60505258-0965-45CE-8FEE-B2C660EAB060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CABE02-EF39-4676-B4E5-734E3E568FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="49">
   <si>
     <t>YEP</t>
   </si>
@@ -173,14 +173,20 @@
     <t>4/10</t>
   </si>
   <si>
-    <t>01/07/2024</t>
+    <t>23/06/2024</t>
+  </si>
+  <si>
+    <t>25/06/2024</t>
+  </si>
+  <si>
+    <t>Mois (en nombre)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -295,8 +301,59 @@
       <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color indexed="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,8 +460,28 @@
         <fgColor rgb="FFFDE6CD"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7B7B7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFF6B26B"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFDE6CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7B7B7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="40">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -644,15 +721,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -675,91 +743,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -788,11 +790,52 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -809,6 +852,28 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -834,6 +899,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -845,11 +936,128 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -865,7 +1073,7 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="16"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="16"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -931,9 +1139,6 @@
     <xf numFmtId="14" fontId="5" fillId="11" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -958,63 +1163,133 @@
     <xf numFmtId="0" fontId="14" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="16" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="16" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="14" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="11" fillId="21" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="21" fillId="22" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="21" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="23" fillId="25" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="25" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="22" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1030,18 +1305,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="26" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1381,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="G97" sqref="G97"/>
+    <sheetView tabSelected="1" topLeftCell="O92" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C112" sqref="C112:AF112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1397,7 +1677,9 @@
     <col min="9" max="9" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="31.21875" customWidth="1"/>
     <col min="11" max="17" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="39" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="24" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="39" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:702 16384:16384" x14ac:dyDescent="0.3">
@@ -1406,10 +1688,10 @@
       </c>
     </row>
     <row r="4" spans="2:702 16384:16384" ht="21" x14ac:dyDescent="0.4">
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="68"/>
+      <c r="D4" s="93"/>
       <c r="G4" s="10">
         <v>20</v>
       </c>
@@ -1422,8 +1704,8 @@
       </c>
     </row>
     <row r="5" spans="2:702 16384:16384" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C5" s="69"/>
-      <c r="D5" s="70"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="95"/>
       <c r="G5" s="12">
         <v>23</v>
       </c>
@@ -1444,48 +1726,93 @@
       <c r="J6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="28">
-        <v>45094</v>
-      </c>
-      <c r="T6" s="28">
-        <v>45461</v>
-      </c>
-      <c r="U6" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="V6" s="42">
-        <v>45828</v>
-      </c>
-      <c r="W6" s="42">
-        <v>46194</v>
-      </c>
-      <c r="X6" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y6" s="42"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="46"/>
+      <c r="Y6" s="41"/>
     </row>
     <row r="7" spans="2:702 16384:16384" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AA7" s="27"/>
+      <c r="C7" s="28">
+        <v>45078</v>
+      </c>
+      <c r="D7" s="28">
+        <v>45079</v>
+      </c>
+      <c r="E7" s="28">
+        <v>45080</v>
+      </c>
+      <c r="F7" s="28">
+        <v>45081</v>
+      </c>
+      <c r="G7" s="28">
+        <v>45082</v>
+      </c>
+      <c r="H7" s="28">
+        <v>45083</v>
+      </c>
+      <c r="I7" s="28">
+        <v>45084</v>
+      </c>
+      <c r="J7" s="28">
+        <v>45085</v>
+      </c>
+      <c r="K7" s="28">
+        <v>45086</v>
+      </c>
+      <c r="L7" s="28">
+        <v>45087</v>
+      </c>
+      <c r="M7" s="28">
+        <v>45088</v>
+      </c>
+      <c r="N7" s="28">
+        <v>45089</v>
+      </c>
+      <c r="O7" s="28">
+        <v>45090</v>
+      </c>
+      <c r="P7" s="28">
+        <v>45091</v>
+      </c>
+      <c r="Q7" s="28">
+        <v>45092</v>
+      </c>
+      <c r="R7" s="28">
+        <v>45093</v>
+      </c>
+      <c r="S7" s="28">
+        <v>45094</v>
+      </c>
+      <c r="T7" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="U7" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" s="41">
+        <v>45828</v>
+      </c>
+      <c r="W7" s="41">
+        <v>46194</v>
+      </c>
+      <c r="X7" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y7" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z7" s="46">
+        <v>45832</v>
+      </c>
+      <c r="AA7" s="74" t="s">
+        <v>47</v>
+      </c>
       <c r="AB7" s="27"/>
       <c r="AC7" s="27"/>
       <c r="AD7" s="27"/>
@@ -2196,7 +2523,7 @@
       </c>
       <c r="S12" s="33"/>
       <c r="T12" s="31"/>
-      <c r="X12" s="39" t="s">
+      <c r="X12" s="38" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2227,541 +2554,604 @@
       </c>
       <c r="S16" s="33"/>
       <c r="T16" s="31"/>
-      <c r="X16" s="39" t="s">
+      <c r="X16" s="38" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:25" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <v>45461.479166666664</v>
       </c>
     </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <v>45461.486111111109</v>
       </c>
     </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <v>45461.493055555555</v>
       </c>
     </row>
-    <row r="20" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:25" ht="18" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <v>45461.5</v>
       </c>
-      <c r="X20" s="51" t="s">
+      <c r="X20" s="48" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y20" s="49" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <v>45461.506944444445</v>
       </c>
     </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <v>45461.513888888891</v>
       </c>
     </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B23" s="2">
         <v>45461.520833333336</v>
       </c>
     </row>
-    <row r="24" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:25" ht="18" x14ac:dyDescent="0.3">
       <c r="B24" s="2">
         <v>45461.527777777781</v>
       </c>
       <c r="X24" s="32" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y24" s="32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B25" s="2">
         <v>45461.534722222219</v>
       </c>
     </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B26" s="2">
         <v>45461.541666666664</v>
       </c>
     </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B27" s="2">
         <v>45461.548611111109</v>
       </c>
     </row>
-    <row r="28" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:25" ht="18" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
         <v>45461.555555555555</v>
       </c>
-      <c r="X28" s="51" t="s">
+      <c r="X28" s="48" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y28" s="32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B29" s="2">
         <v>45461.5625</v>
       </c>
     </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B30" s="2">
         <v>45461.569444444445</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:25" x14ac:dyDescent="0.3">
       <c r="B31" s="2">
         <v>45461.576388888891</v>
       </c>
     </row>
-    <row r="32" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:25" ht="18" x14ac:dyDescent="0.3">
       <c r="B32" s="2">
         <v>45461.583333333336</v>
       </c>
-      <c r="X32" s="52" t="s">
+      <c r="X32" s="49" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y32" s="32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>45461.590277777781</v>
       </c>
       <c r="S33" s="33"/>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>45461.597222222219</v>
       </c>
       <c r="S34" s="33"/>
       <c r="T34" s="31"/>
     </row>
-    <row r="35" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>45461.604166666664</v>
       </c>
       <c r="S35" s="33"/>
       <c r="T35" s="31"/>
     </row>
-    <row r="36" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:27" ht="18" x14ac:dyDescent="0.3">
       <c r="B36" s="2">
         <v>45461.611111111109</v>
       </c>
       <c r="S36" s="33"/>
       <c r="T36" s="31"/>
-      <c r="X36" s="51" t="s">
+      <c r="X36" s="48" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="37" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y36" s="44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>45461.618055555555</v>
       </c>
       <c r="S37" s="33"/>
       <c r="T37" s="31"/>
     </row>
-    <row r="38" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>45461.625</v>
       </c>
       <c r="S38" s="33"/>
       <c r="T38" s="31"/>
     </row>
-    <row r="39" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>45461.631944444445</v>
       </c>
       <c r="S39" s="33"/>
       <c r="T39" s="31"/>
     </row>
-    <row r="40" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:27" ht="18" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>45461.638888888891</v>
       </c>
       <c r="S40" s="33"/>
       <c r="T40" s="31"/>
-      <c r="X40" s="51" t="s">
+      <c r="X40" s="48" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="41" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y40" s="48" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>45461.645833333336</v>
       </c>
       <c r="S41" s="33"/>
       <c r="T41" s="31"/>
     </row>
-    <row r="42" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B42" s="2">
         <v>45461.652777777781</v>
       </c>
       <c r="S42" s="33"/>
       <c r="T42" s="31"/>
     </row>
-    <row r="43" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>45461.659722222219</v>
       </c>
       <c r="S43" s="33"/>
       <c r="T43" s="31"/>
     </row>
-    <row r="44" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:27" ht="18" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
         <v>45461.666666666664</v>
       </c>
       <c r="S44" s="33"/>
       <c r="T44" s="31"/>
-      <c r="X44" s="45" t="s">
+      <c r="X44" s="44" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="45" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="Y44" s="73" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>45461.673611111109</v>
       </c>
       <c r="S45" s="33"/>
       <c r="T45" s="31"/>
     </row>
-    <row r="46" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
         <v>45461.680555555555</v>
       </c>
       <c r="S46" s="33"/>
       <c r="T46" s="31"/>
     </row>
-    <row r="47" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B47" s="2">
         <v>45461.6875</v>
       </c>
       <c r="S47" s="33"/>
       <c r="T47" s="31"/>
     </row>
-    <row r="48" spans="2:24" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B48" s="2">
         <v>45461.694444444445</v>
       </c>
-      <c r="I48" s="44"/>
+      <c r="I48" s="43"/>
       <c r="S48" s="32" t="s">
         <v>32</v>
       </c>
       <c r="T48" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="U48" s="44" t="s">
+      <c r="U48" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="X48" s="52" t="s">
+      <c r="X48" s="49" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="49" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y48" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA48" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="2:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
         <v>45461.701388888891</v>
       </c>
       <c r="S49" s="31"/>
       <c r="T49" s="31"/>
     </row>
-    <row r="50" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B50" s="2">
         <v>45461.708333333336</v>
       </c>
       <c r="S50" s="31"/>
       <c r="T50" s="31"/>
     </row>
-    <row r="51" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="2">
         <v>45461.715277777781</v>
       </c>
       <c r="S51" s="31"/>
       <c r="T51" s="31"/>
     </row>
-    <row r="52" spans="2:24" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="2">
         <v>45461.722222222219</v>
       </c>
-      <c r="I52" s="44"/>
+      <c r="I52" s="43"/>
       <c r="S52" s="32" t="s">
         <v>32</v>
       </c>
       <c r="T52" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="U52" s="44" t="s">
+      <c r="U52" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="X52" s="52" t="s">
+      <c r="X52" s="49" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="53" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y52" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA52" s="38" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="2:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B53" s="2">
         <v>45461.729166666664</v>
       </c>
       <c r="S53" s="31"/>
       <c r="T53" s="31"/>
     </row>
-    <row r="54" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B54" s="2">
         <v>45461.736111111109</v>
       </c>
       <c r="S54" s="31"/>
       <c r="T54" s="31"/>
     </row>
-    <row r="55" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="2">
         <v>45461.743055555555</v>
       </c>
       <c r="S55" s="31"/>
       <c r="T55" s="31"/>
     </row>
-    <row r="56" spans="2:24" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="2">
         <v>45461.75</v>
       </c>
-      <c r="I56" s="44"/>
-      <c r="S56" s="38" t="s">
+      <c r="I56" s="43"/>
+      <c r="S56" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="T56" s="38" t="s">
+      <c r="T56" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="U56" s="39" t="s">
+      <c r="U56" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="X56" s="51" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="57" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="X56" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y56" s="32" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA56" s="45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="2:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B57" s="2">
         <v>45461.756944444445</v>
       </c>
       <c r="S57" s="31"/>
       <c r="T57" s="31"/>
     </row>
-    <row r="58" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:27" x14ac:dyDescent="0.3">
       <c r="B58" s="2">
         <v>45461.763888888891</v>
       </c>
       <c r="S58" s="31"/>
       <c r="T58" s="31"/>
     </row>
-    <row r="59" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B59" s="2">
         <v>45461.770833333336</v>
       </c>
       <c r="S59" s="31"/>
       <c r="T59" s="31"/>
     </row>
-    <row r="60" spans="2:24" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B60" s="2">
         <v>45461.777777777781</v>
       </c>
-      <c r="I60" s="44"/>
-      <c r="S60" s="38" t="s">
+      <c r="I60" s="43"/>
+      <c r="S60" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="T60" s="38" t="s">
+      <c r="T60" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="X60" s="45" t="s">
+      <c r="X60" s="44" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="61" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Y60" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA60" s="45" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="2:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B61" s="2">
         <v>45461.784722222219</v>
       </c>
       <c r="S61" s="31"/>
       <c r="T61" s="31"/>
     </row>
-    <row r="62" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:27" ht="18" x14ac:dyDescent="0.3">
       <c r="B62" s="2">
         <v>45461.791666666664</v>
       </c>
       <c r="S62" s="31"/>
       <c r="T62" s="31"/>
-      <c r="U62" s="45" t="s">
+      <c r="U62" s="44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="63" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="2">
         <v>45461.798611111109</v>
       </c>
       <c r="S63" s="31"/>
       <c r="T63" s="31"/>
     </row>
-    <row r="64" spans="2:24" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B64" s="2">
         <v>45461.805555555555</v>
       </c>
-      <c r="I64" s="44"/>
-      <c r="S64" s="39" t="s">
+      <c r="I64" s="43"/>
+      <c r="S64" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="T64" s="39" t="s">
+      <c r="T64" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="X64" s="51" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="65" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="X64" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y64" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA64" s="38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="65" spans="2:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B65" s="2">
         <v>45461.8125</v>
       </c>
       <c r="S65" s="31"/>
       <c r="T65" s="31"/>
     </row>
-    <row r="66" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:27" ht="18" x14ac:dyDescent="0.3">
       <c r="B66" s="2">
         <v>45461.819444444445</v>
       </c>
       <c r="S66" s="31"/>
       <c r="T66" s="31"/>
-      <c r="U66" s="45" t="s">
+      <c r="U66" s="44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B67" s="2">
         <v>45461.826388888891</v>
       </c>
       <c r="S67" s="31"/>
       <c r="T67" s="31"/>
     </row>
-    <row r="68" spans="2:24" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B68" s="2">
         <v>45461.833333333336</v>
       </c>
-      <c r="I68" s="44"/>
-      <c r="S68" s="39" t="s">
+      <c r="I68" s="43"/>
+      <c r="S68" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="T68" s="39" t="s">
+      <c r="T68" s="38" t="s">
         <v>36</v>
       </c>
       <c r="X68" s="32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="69" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AA68" s="37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="69" spans="2:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B69" s="2">
         <v>45461.840277777781</v>
       </c>
       <c r="S69" s="31"/>
       <c r="T69" s="31"/>
     </row>
-    <row r="70" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:27" ht="18" x14ac:dyDescent="0.3">
       <c r="B70" s="2">
         <v>45461.847222222219</v>
       </c>
       <c r="S70" s="31"/>
       <c r="T70" s="31"/>
-      <c r="U70" s="45" t="s">
+      <c r="U70" s="44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="71" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B71" s="2">
         <v>45461.854166666664</v>
       </c>
       <c r="S71" s="31"/>
       <c r="T71" s="31"/>
     </row>
-    <row r="72" spans="2:24" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:27" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B72" s="2">
         <v>45461.861111111109</v>
       </c>
-      <c r="I72" s="44"/>
-      <c r="S72" s="40" t="s">
+      <c r="I72" s="43"/>
+      <c r="S72" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="T72" s="40" t="s">
+      <c r="T72" s="39" t="s">
         <v>34</v>
       </c>
       <c r="X72" s="32" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="73" spans="2:24" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AA72" s="43" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="73" spans="2:27" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B73" s="2">
         <v>45461.868055555555</v>
       </c>
       <c r="S73" s="31"/>
       <c r="T73" s="31"/>
     </row>
-    <row r="74" spans="2:24" ht="18" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:27" ht="18" x14ac:dyDescent="0.3">
       <c r="B74" s="2">
         <v>45461.875</v>
       </c>
       <c r="S74" s="31"/>
       <c r="T74" s="31"/>
-      <c r="U74" s="45" t="s">
+      <c r="U74" s="44" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="75" spans="2:24" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B75" s="2">
         <v>45461.881944444445</v>
       </c>
       <c r="S75" s="31"/>
       <c r="T75" s="31"/>
     </row>
-    <row r="76" spans="2:24" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:27" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B76" s="2">
         <v>45461.888888888891</v>
       </c>
-      <c r="I76" s="44"/>
-      <c r="S76" s="41" t="s">
+      <c r="I76" s="43"/>
+      <c r="S76" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="T76" s="41" t="s">
+      <c r="T76" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="X76" s="52" t="s">
+      <c r="X76" s="49" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="77" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA76" s="38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="2:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B77" s="2">
         <v>45461.895833333336</v>
       </c>
       <c r="S77" s="31"/>
       <c r="T77" s="31"/>
     </row>
-    <row r="78" spans="2:24" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:27" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B78" s="2">
         <v>45461.902777777781</v>
       </c>
       <c r="S78" s="31"/>
       <c r="T78" s="31"/>
-      <c r="U78" s="46" t="s">
+      <c r="U78" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="79" spans="2:24" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:27" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="2">
         <v>45461.909722222219</v>
       </c>
       <c r="S79" s="31"/>
       <c r="T79" s="31"/>
     </row>
-    <row r="80" spans="2:24" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:27" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B80" s="2">
         <v>45461.916666666664</v>
       </c>
-      <c r="I80" s="39"/>
-      <c r="S80" s="41" t="s">
+      <c r="I80" s="38"/>
+      <c r="S80" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="T80" s="41" t="s">
+      <c r="T80" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="X80" s="45" t="s">
+      <c r="X80" s="44" t="s">
         <v>39</v>
+      </c>
+      <c r="AA80" s="38" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="81" spans="2:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2777,7 +3167,7 @@
       </c>
       <c r="S82" s="31"/>
       <c r="T82" s="31"/>
-      <c r="U82" s="39" t="s">
+      <c r="U82" s="38" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2792,15 +3182,18 @@
       <c r="B84" s="2">
         <v>45461.944444444445</v>
       </c>
-      <c r="I84" s="39"/>
-      <c r="S84" s="41" t="s">
+      <c r="I84" s="38"/>
+      <c r="S84" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="T84" s="41" t="s">
+      <c r="T84" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="X84" s="32" t="s">
-        <v>42</v>
+      <c r="X84" s="44" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA84" s="38" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="85" spans="2:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -2816,7 +3209,7 @@
       </c>
       <c r="S86" s="33"/>
       <c r="T86" s="31"/>
-      <c r="U86" s="39" t="s">
+      <c r="U86" s="38" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2831,7 +3224,7 @@
       <c r="B88" s="2">
         <v>45461.972222222219</v>
       </c>
-      <c r="I88" s="58"/>
+      <c r="I88" s="53"/>
       <c r="S88" s="33"/>
       <c r="T88" s="31"/>
       <c r="X88" s="32" t="s">
@@ -2865,7 +3258,7 @@
       </c>
       <c r="S92" s="33"/>
       <c r="T92" s="31"/>
-      <c r="X92" s="44" t="s">
+      <c r="X92" s="43" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2927,281 +3320,466 @@
       <c r="T93" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="U93" s="43" t="s">
+      <c r="U93" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="V93" s="53">
+      <c r="V93" s="50">
         <v>45828</v>
       </c>
-      <c r="W93" s="53">
+      <c r="W93" s="50">
         <v>46194</v>
       </c>
-      <c r="X93" s="49" t="s">
+      <c r="X93" s="47" t="s">
         <v>40</v>
+      </c>
+      <c r="Y93" s="60" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z93" s="79">
+        <v>45832</v>
+      </c>
+      <c r="AA93" s="75" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="94" spans="2:39" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B94" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="I94" s="35"/>
-      <c r="J94" s="55"/>
-      <c r="K94" s="60"/>
-      <c r="S94" s="35">
+      <c r="C94" s="64"/>
+      <c r="D94" s="64"/>
+      <c r="E94" s="64"/>
+      <c r="F94" s="64"/>
+      <c r="G94" s="64"/>
+      <c r="H94" s="64"/>
+      <c r="I94" s="65"/>
+      <c r="J94" s="64"/>
+      <c r="K94" s="64"/>
+      <c r="L94" s="64"/>
+      <c r="M94" s="64"/>
+      <c r="N94" s="64"/>
+      <c r="O94" s="64"/>
+      <c r="P94" s="64"/>
+      <c r="Q94" s="64"/>
+      <c r="R94" s="64"/>
+      <c r="S94" s="65">
         <v>0.41379310344827586</v>
       </c>
-      <c r="T94" s="35">
+      <c r="T94" s="65">
         <v>0.41379310344827586</v>
       </c>
-      <c r="U94" s="35">
+      <c r="U94" s="65">
         <v>0.76595744680851063</v>
       </c>
-      <c r="V94" s="54">
-        <v>0.5</v>
-      </c>
-      <c r="W94" s="50">
-        <v>0.5</v>
-      </c>
-      <c r="X94" s="35">
-        <v>0.62135922330097093</v>
-      </c>
+      <c r="V94" s="66"/>
+      <c r="W94" s="67"/>
+      <c r="X94" s="65">
+        <v>0.68932038834951459</v>
+      </c>
+      <c r="Y94" s="71">
+        <v>0.38333333333333336</v>
+      </c>
+      <c r="Z94" s="64"/>
+      <c r="AA94" s="71">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="AB94" s="64"/>
+      <c r="AC94" s="81"/>
+      <c r="AD94" s="64"/>
+      <c r="AE94" s="64"/>
+      <c r="AF94" s="64"/>
     </row>
     <row r="95" spans="2:39" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="I95" s="59"/>
-      <c r="J95" s="59"/>
-      <c r="K95" s="62"/>
-      <c r="L95" s="59"/>
-      <c r="M95" s="59"/>
-      <c r="N95" s="59"/>
-      <c r="O95" s="59"/>
-      <c r="P95" s="59"/>
-      <c r="Q95" s="59"/>
-      <c r="R95" s="59"/>
-      <c r="S95" s="74">
-        <v>0.59682916752737047</v>
-      </c>
-      <c r="T95" s="75"/>
-      <c r="U95" s="75"/>
-      <c r="V95" s="75"/>
-      <c r="W95" s="75"/>
-      <c r="X95" s="76"/>
-      <c r="AD95" s="59"/>
-      <c r="AE95" s="59"/>
-      <c r="AF95" s="59"/>
-      <c r="AG95" s="59"/>
-      <c r="AH95" s="59"/>
-      <c r="AI95" s="59"/>
-      <c r="AJ95" s="59"/>
-      <c r="AK95" s="59"/>
-      <c r="AL95" s="59"/>
-      <c r="AM95" s="59"/>
+      <c r="C95" s="76"/>
+      <c r="D95" s="68"/>
+      <c r="E95" s="68"/>
+      <c r="F95" s="68"/>
+      <c r="G95" s="68"/>
+      <c r="H95" s="68"/>
+      <c r="I95" s="69"/>
+      <c r="J95" s="69"/>
+      <c r="K95" s="70"/>
+      <c r="L95" s="69"/>
+      <c r="M95" s="69"/>
+      <c r="N95" s="69"/>
+      <c r="O95" s="69"/>
+      <c r="P95" s="69"/>
+      <c r="Q95" s="69"/>
+      <c r="R95" s="69"/>
+      <c r="S95" s="99">
+        <v>0.76595744680851097</v>
+      </c>
+      <c r="T95" s="100"/>
+      <c r="U95" s="100"/>
+      <c r="V95" s="100"/>
+      <c r="W95" s="100"/>
+      <c r="X95" s="100"/>
+      <c r="Y95" s="101">
+        <v>0.38333333333333303</v>
+      </c>
+      <c r="Z95" s="103">
+        <v>0.86666666666666703</v>
+      </c>
+      <c r="AA95" s="103"/>
+      <c r="AB95" s="103"/>
+      <c r="AC95" s="103"/>
+      <c r="AD95" s="104"/>
+      <c r="AE95" s="104"/>
+      <c r="AF95" s="69"/>
+      <c r="AG95" s="63"/>
+      <c r="AH95" s="54"/>
+      <c r="AI95" s="54"/>
+      <c r="AJ95" s="54"/>
+      <c r="AK95" s="54"/>
+      <c r="AL95" s="54"/>
+      <c r="AM95" s="54"/>
     </row>
     <row r="96" spans="2:39" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="16" t="s">
+      <c r="B96" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C96" s="78"/>
-      <c r="D96" s="78"/>
-      <c r="E96" s="78"/>
-      <c r="F96" s="78"/>
-      <c r="G96" s="78"/>
-      <c r="H96" s="78"/>
-      <c r="I96" s="78"/>
-      <c r="J96" s="78"/>
-      <c r="K96" s="78"/>
-      <c r="L96" s="78"/>
-      <c r="M96" s="78"/>
-      <c r="N96" s="78"/>
-      <c r="O96" s="78"/>
-      <c r="P96" s="78"/>
-      <c r="Q96" s="78"/>
-      <c r="R96" s="78"/>
-      <c r="S96" s="78"/>
-      <c r="T96" s="78"/>
-      <c r="U96" s="78"/>
-      <c r="V96" s="78"/>
-      <c r="W96" s="78"/>
-      <c r="X96" s="78"/>
-      <c r="Y96" s="78"/>
-      <c r="Z96" s="78"/>
-      <c r="AA96" s="78"/>
-      <c r="AB96" s="78"/>
-      <c r="AC96" s="78"/>
-      <c r="AD96" s="78"/>
-      <c r="AE96" s="78"/>
-      <c r="AF96" s="78"/>
-      <c r="AG96" s="77"/>
-      <c r="AH96" s="77"/>
-      <c r="AI96" s="77"/>
-      <c r="AJ96" s="77"/>
-      <c r="AK96" s="77"/>
-      <c r="AL96" s="77"/>
-      <c r="AM96" s="77"/>
-    </row>
-    <row r="97" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C96" s="84">
+        <v>0.67198581560283699</v>
+      </c>
+      <c r="D96" s="85"/>
+      <c r="E96" s="86"/>
+      <c r="F96" s="86"/>
+      <c r="G96" s="86"/>
+      <c r="H96" s="86"/>
+      <c r="I96" s="86"/>
+      <c r="J96" s="86"/>
+      <c r="K96" s="86"/>
+      <c r="L96" s="86"/>
+      <c r="M96" s="86"/>
+      <c r="N96" s="86"/>
+      <c r="O96" s="86"/>
+      <c r="P96" s="86"/>
+      <c r="Q96" s="86"/>
+      <c r="R96" s="86"/>
+      <c r="S96" s="86"/>
+      <c r="T96" s="86"/>
+      <c r="U96" s="86"/>
+      <c r="V96" s="86"/>
+      <c r="W96" s="86"/>
+      <c r="X96" s="86"/>
+      <c r="Y96" s="86"/>
+      <c r="Z96" s="86"/>
+      <c r="AA96" s="86"/>
+      <c r="AB96" s="86"/>
+      <c r="AC96" s="86"/>
+      <c r="AD96" s="86"/>
+      <c r="AE96" s="86"/>
+      <c r="AF96" s="87"/>
+      <c r="AG96" s="64"/>
+    </row>
+    <row r="97" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B98" s="17" t="s">
         <v>13</v>
       </c>
       <c r="C98" s="17"/>
     </row>
-    <row r="99" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B99" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C99" s="30">
+      <c r="J99" s="51"/>
+      <c r="K99" s="55"/>
+      <c r="R99" s="35"/>
+      <c r="S99" s="30">
         <v>58</v>
       </c>
-      <c r="D99" s="36">
+      <c r="T99" s="35">
         <v>58</v>
       </c>
-      <c r="E99" s="36">
-        <v>94</v>
-      </c>
-      <c r="F99" s="30">
+      <c r="U99" s="35">
+        <v>206</v>
+      </c>
+      <c r="V99" s="61">
         <v>0</v>
       </c>
-      <c r="G99" s="30">
+      <c r="W99" s="35">
+        <v>96</v>
+      </c>
+      <c r="X99" s="57">
+        <v>206</v>
+      </c>
+      <c r="Y99" s="35">
+        <v>120</v>
+      </c>
+      <c r="Z99" s="77">
         <v>0</v>
       </c>
-      <c r="H99" s="36">
-        <v>206</v>
-      </c>
-      <c r="I99" s="36">
-        <v>96</v>
-      </c>
-      <c r="J99" s="56"/>
-      <c r="K99" s="60"/>
-    </row>
-    <row r="100" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AA99" s="35">
+        <v>90</v>
+      </c>
+      <c r="AC99" s="81"/>
+    </row>
+    <row r="100" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C100" s="30">
+      <c r="J100" s="51"/>
+      <c r="K100" s="55"/>
+      <c r="Q100" s="30"/>
+      <c r="R100" s="30"/>
+      <c r="S100" s="30">
         <v>24</v>
       </c>
-      <c r="D100" s="36">
+      <c r="T100" s="35">
         <v>24</v>
       </c>
-      <c r="E100" s="36">
-        <v>72</v>
-      </c>
-      <c r="F100" s="30">
+      <c r="U100" s="35">
+        <v>128</v>
+      </c>
+      <c r="V100" s="62">
         <v>0</v>
       </c>
-      <c r="G100" s="30">
+      <c r="W100" s="35">
+        <v>2</v>
+      </c>
+      <c r="X100" s="57">
+        <v>142</v>
+      </c>
+      <c r="Y100" s="35">
+        <v>46</v>
+      </c>
+      <c r="Z100" s="77">
         <v>0</v>
       </c>
-      <c r="H100" s="36">
-        <v>128</v>
-      </c>
-      <c r="I100" s="36">
-        <v>2</v>
-      </c>
-      <c r="J100" s="56"/>
-      <c r="K100" s="60"/>
-    </row>
-    <row r="101" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="71" t="s">
+      <c r="AA100" s="35">
+        <v>78</v>
+      </c>
+      <c r="AC100" s="81"/>
+    </row>
+    <row r="101" spans="1:32" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="96" t="s">
         <v>16</v>
       </c>
-      <c r="B101" s="72"/>
-    </row>
-    <row r="102" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="73" t="s">
+      <c r="B101" s="97"/>
+    </row>
+    <row r="102" spans="1:32" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="98" t="s">
         <v>17</v>
       </c>
-      <c r="B102" s="72"/>
-    </row>
-    <row r="104" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="73" t="s">
+      <c r="B102" s="97"/>
+      <c r="C102" s="72">
+        <v>0.67198581560283699</v>
+      </c>
+      <c r="D102" s="72"/>
+    </row>
+    <row r="103" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="B103" s="80" t="s">
+        <v>48</v>
+      </c>
+      <c r="C103" s="80">
+        <v>6</v>
+      </c>
+      <c r="D103" s="80"/>
+      <c r="E103" s="80"/>
+    </row>
+    <row r="104" spans="1:32" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="98" t="s">
         <v>18</v>
       </c>
-      <c r="B104" s="72"/>
-    </row>
-    <row r="106" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="107" spans="1:11" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C107" s="47">
+      <c r="B104" s="97"/>
+    </row>
+    <row r="106" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="107" spans="1:32" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C107" s="34">
+        <v>45078</v>
+      </c>
+      <c r="D107" s="34">
+        <v>45079</v>
+      </c>
+      <c r="E107" s="34">
+        <v>45080</v>
+      </c>
+      <c r="F107" s="34">
+        <v>45081</v>
+      </c>
+      <c r="G107" s="34">
+        <v>45082</v>
+      </c>
+      <c r="H107" s="34">
+        <v>45083</v>
+      </c>
+      <c r="I107" s="34">
+        <v>45084</v>
+      </c>
+      <c r="J107" s="34">
+        <v>45085</v>
+      </c>
+      <c r="K107" s="34">
+        <v>45086</v>
+      </c>
+      <c r="L107" s="34">
+        <v>45087</v>
+      </c>
+      <c r="M107" s="34">
+        <v>45088</v>
+      </c>
+      <c r="N107" s="34">
+        <v>45089</v>
+      </c>
+      <c r="O107" s="34">
+        <v>45090</v>
+      </c>
+      <c r="P107" s="34">
+        <v>45091</v>
+      </c>
+      <c r="Q107" s="34">
+        <v>45092</v>
+      </c>
+      <c r="R107" s="34">
+        <v>45093</v>
+      </c>
+      <c r="S107" s="34">
         <v>45094</v>
       </c>
-      <c r="D107" s="29" t="s">
+      <c r="T107" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E107" s="43" t="s">
+      <c r="U107" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F107" s="53">
+      <c r="V107" s="50">
         <v>45828</v>
       </c>
-      <c r="G107" s="53">
+      <c r="W107" s="50">
         <v>46194</v>
       </c>
-      <c r="H107" s="49" t="s">
+      <c r="X107" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="I107" s="43" t="s">
+      <c r="Y107" s="60" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="108" spans="1:11" s="21" customFormat="1" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="Z107" s="79">
+        <v>45832</v>
+      </c>
+      <c r="AA107" s="75" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="108" spans="1:32" s="21" customFormat="1" ht="19.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
       <c r="B108" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C108" s="37">
+      <c r="C108" s="83"/>
+      <c r="J108" s="52"/>
+      <c r="K108" s="56"/>
+      <c r="N108" s="36">
         <v>440</v>
       </c>
-      <c r="D108" s="37">
+      <c r="O108" s="36">
         <v>480</v>
       </c>
-      <c r="E108" s="37">
+      <c r="P108" s="36">
         <f>(2+4+10+10+10+10+10+8+8)*20</f>
         <v>1440</v>
       </c>
-      <c r="F108" s="37">
+      <c r="Q108" s="36">
         <v>0</v>
       </c>
-      <c r="G108" s="37">
+      <c r="R108" s="36">
         <v>0</v>
       </c>
-      <c r="H108" s="37">
+      <c r="S108" s="36">
         <v>2896</v>
       </c>
-      <c r="I108" s="37">
-        <v>40</v>
-      </c>
-      <c r="J108" s="57"/>
-      <c r="K108" s="61"/>
-    </row>
-    <row r="110" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A110">
-        <v>5072</v>
-      </c>
+      <c r="T108" s="36"/>
+      <c r="X108" s="58">
+        <v>3218</v>
+      </c>
+      <c r="Y108" s="36">
+        <v>1058</v>
+      </c>
+      <c r="AA108" s="36">
+        <v>1560</v>
+      </c>
+      <c r="AC108" s="82"/>
+    </row>
+    <row r="109" spans="1:32" ht="23.4" x14ac:dyDescent="0.3">
+      <c r="M109" s="88">
+        <v>5256</v>
+      </c>
+      <c r="N109" s="89"/>
+      <c r="O109" s="89"/>
+      <c r="P109" s="90"/>
+      <c r="Q109" s="89"/>
+      <c r="R109" s="89"/>
+      <c r="S109" s="91"/>
+    </row>
+    <row r="110" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C110" s="63">
-        <v>5256</v>
-      </c>
-      <c r="D110" s="64"/>
-      <c r="E110" s="64"/>
-      <c r="F110" s="65"/>
-      <c r="G110" s="64"/>
-      <c r="H110" s="64"/>
-      <c r="I110" s="66"/>
-      <c r="J110" s="56"/>
-      <c r="K110" s="60"/>
-    </row>
-    <row r="112" spans="1:11" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J110" s="51"/>
+      <c r="K110" s="55"/>
+      <c r="S110" s="102">
+        <v>4276</v>
+      </c>
+      <c r="T110" s="102"/>
+      <c r="U110" s="102"/>
+      <c r="V110" s="102"/>
+      <c r="W110" s="102"/>
+      <c r="X110" s="102"/>
+      <c r="Y110" s="102">
+        <v>1058</v>
+      </c>
+      <c r="Z110" s="102">
+        <v>1560</v>
+      </c>
+      <c r="AA110" s="97"/>
+      <c r="AB110" s="97"/>
+      <c r="AC110" s="97"/>
+      <c r="AD110" s="97"/>
+      <c r="AE110" s="97"/>
+    </row>
+    <row r="112" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="20" t="s">
         <v>21</v>
       </c>
+      <c r="C112" s="102">
+        <v>11092</v>
+      </c>
+      <c r="D112" s="102"/>
+      <c r="E112" s="102"/>
+      <c r="F112" s="102"/>
+      <c r="G112" s="102"/>
+      <c r="H112" s="102"/>
+      <c r="I112" s="102"/>
+      <c r="J112" s="102"/>
+      <c r="K112" s="102"/>
+      <c r="L112" s="102"/>
+      <c r="M112" s="102"/>
+      <c r="N112" s="102"/>
+      <c r="O112" s="102"/>
+      <c r="P112" s="102"/>
+      <c r="Q112" s="102"/>
+      <c r="R112" s="102"/>
+      <c r="S112" s="102"/>
+      <c r="T112" s="102"/>
+      <c r="U112" s="102"/>
+      <c r="V112" s="102"/>
+      <c r="W112" s="102"/>
+      <c r="X112" s="102"/>
+      <c r="Y112" s="102"/>
+      <c r="Z112" s="102"/>
+      <c r="AA112" s="102"/>
+      <c r="AB112" s="102"/>
+      <c r="AC112" s="102"/>
+      <c r="AD112" s="102"/>
+      <c r="AE112" s="102"/>
+      <c r="AF112" s="102"/>
     </row>
     <row r="114" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="20" t="s">
@@ -3249,16 +3827,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="S95:X95"/>
+  <mergeCells count="11">
+    <mergeCell ref="C112:AF112"/>
     <mergeCell ref="C96:AF96"/>
-    <mergeCell ref="C110:I110"/>
+    <mergeCell ref="M109:S109"/>
     <mergeCell ref="C4:D5"/>
     <mergeCell ref="A101:B101"/>
     <mergeCell ref="A102:B102"/>
     <mergeCell ref="A104:B104"/>
+    <mergeCell ref="S95:Y95"/>
+    <mergeCell ref="S110:Y110"/>
+    <mergeCell ref="Z95:AE95"/>
+    <mergeCell ref="Z110:AE110"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CA + TR ok avec tickets vendus / mois ok
</commit_message>
<xml_diff>
--- a/dataFormatts.xlsx
+++ b/dataFormatts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Stage\AllWebScraping_VirtualGame\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CABE02-EF39-4676-B4E5-734E3E568FBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62368E51-3802-47F8-A6B0-5CE4348DAAC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -353,7 +353,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,8 +480,14 @@
         <fgColor rgb="FFB7B7B7"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="51">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -772,21 +778,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF00FF02"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF00FF02"/>
-      </right>
-      <top style="thick">
-        <color rgb="FF00FF02"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FF00FF02"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -1067,13 +1058,149 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color theme="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color theme="1"/>
+      </top>
+      <bottom style="thick">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="16"/>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="16"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1157,9 +1284,6 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="15" fontId="14" fillId="15" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1170,9 +1294,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="16" fillId="18" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="18" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1189,107 +1310,111 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="21" fillId="22" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="21" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="18" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="11" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="23" fillId="25" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="25" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="22" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="20" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="21" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="11" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="23" fillId="25" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="25" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="22" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="22" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="10" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="22" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="37" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="37" fontId="22" fillId="0" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1305,22 +1430,55 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="17" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="26" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="17" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="26" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyBorder="1"/>
+    <xf numFmtId="15" fontId="5" fillId="11" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="16" fillId="18" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="26" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="14" fillId="26" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="14" fillId="26" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="16" fillId="26" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="11" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="14" fillId="15" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="16" fillId="18" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="21" fillId="22" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="5" fillId="11" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1661,15 +1819,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O92" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C112" sqref="C112:AF112"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" customWidth="1"/>
     <col min="2" max="2" width="35.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
     <col min="4" max="4" width="17.44140625" customWidth="1"/>
     <col min="5" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="11.6640625" customWidth="1"/>
@@ -1687,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:702 16384:16384" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:702 16384:16384" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="C4" s="92" t="s">
         <v>8</v>
       </c>
@@ -1716,6 +1874,8 @@
       <c r="J5" s="8" t="s">
         <v>3</v>
       </c>
+      <c r="S5" s="106"/>
+      <c r="T5" s="105"/>
     </row>
     <row r="6" spans="2:702 16384:16384" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="G6" s="14"/>
@@ -1726,13 +1886,14 @@
       <c r="J6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="41"/>
-      <c r="V6" s="41"/>
-      <c r="W6" s="41"/>
-      <c r="X6" s="46"/>
-      <c r="Y6" s="41"/>
+      <c r="R6" s="105"/>
+      <c r="S6" s="109"/>
+      <c r="T6" s="109"/>
+      <c r="U6" s="110"/>
+      <c r="V6" s="111"/>
+      <c r="W6" s="111"/>
+      <c r="X6" s="112"/>
+      <c r="Y6" s="110"/>
     </row>
     <row r="7" spans="2:702 16384:16384" ht="15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
@@ -1780,37 +1941,37 @@
       <c r="P7" s="28">
         <v>45091</v>
       </c>
-      <c r="Q7" s="28">
+      <c r="Q7" s="107">
         <v>45092</v>
       </c>
-      <c r="R7" s="28">
+      <c r="R7" s="113">
         <v>45093</v>
       </c>
-      <c r="S7" s="28">
+      <c r="S7" s="113">
         <v>45094</v>
       </c>
-      <c r="T7" s="28" t="s">
+      <c r="T7" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="U7" s="41" t="s">
+      <c r="U7" s="114" t="s">
         <v>37</v>
       </c>
-      <c r="V7" s="41">
+      <c r="V7" s="114">
         <v>45828</v>
       </c>
-      <c r="W7" s="41">
+      <c r="W7" s="114">
         <v>46194</v>
       </c>
-      <c r="X7" s="46" t="s">
+      <c r="X7" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="Y7" s="59" t="s">
+      <c r="Y7" s="116" t="s">
         <v>46</v>
       </c>
-      <c r="Z7" s="46">
+      <c r="Z7" s="108">
         <v>45832</v>
       </c>
-      <c r="AA7" s="74" t="s">
+      <c r="AA7" s="70" t="s">
         <v>47</v>
       </c>
       <c r="AB7" s="27"/>
@@ -2577,10 +2738,10 @@
       <c r="B20" s="2">
         <v>45461.5</v>
       </c>
-      <c r="X20" s="48" t="s">
+      <c r="X20" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="Y20" s="49" t="s">
+      <c r="Y20" s="47" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2629,7 +2790,7 @@
       <c r="B28" s="2">
         <v>45461.555555555555</v>
       </c>
-      <c r="X28" s="48" t="s">
+      <c r="X28" s="46" t="s">
         <v>41</v>
       </c>
       <c r="Y28" s="32" t="s">
@@ -2655,7 +2816,7 @@
       <c r="B32" s="2">
         <v>45461.583333333336</v>
       </c>
-      <c r="X32" s="49" t="s">
+      <c r="X32" s="47" t="s">
         <v>35</v>
       </c>
       <c r="Y32" s="32" t="s">
@@ -2689,10 +2850,10 @@
       </c>
       <c r="S36" s="33"/>
       <c r="T36" s="31"/>
-      <c r="X36" s="48" t="s">
+      <c r="X36" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="Y36" s="44" t="s">
+      <c r="Y36" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2723,10 +2884,10 @@
       </c>
       <c r="S40" s="33"/>
       <c r="T40" s="31"/>
-      <c r="X40" s="48" t="s">
+      <c r="X40" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="Y40" s="48" t="s">
+      <c r="Y40" s="46" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2757,10 +2918,10 @@
       </c>
       <c r="S44" s="33"/>
       <c r="T44" s="31"/>
-      <c r="X44" s="44" t="s">
+      <c r="X44" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="Y44" s="73" t="s">
+      <c r="Y44" s="69" t="s">
         <v>44</v>
       </c>
     </row>
@@ -2789,17 +2950,16 @@
       <c r="B48" s="2">
         <v>45461.694444444445</v>
       </c>
-      <c r="I48" s="43"/>
       <c r="S48" s="32" t="s">
         <v>32</v>
       </c>
       <c r="T48" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="U48" s="43" t="s">
+      <c r="U48" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="X48" s="49" t="s">
+      <c r="X48" s="47" t="s">
         <v>39</v>
       </c>
       <c r="Y48" s="32" t="s">
@@ -2834,17 +2994,16 @@
       <c r="B52" s="2">
         <v>45461.722222222219</v>
       </c>
-      <c r="I52" s="43"/>
       <c r="S52" s="32" t="s">
         <v>32</v>
       </c>
       <c r="T52" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="U52" s="43" t="s">
+      <c r="U52" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="X52" s="49" t="s">
+      <c r="X52" s="47" t="s">
         <v>33</v>
       </c>
       <c r="Y52" s="32" t="s">
@@ -2879,7 +3038,6 @@
       <c r="B56" s="2">
         <v>45461.75</v>
       </c>
-      <c r="I56" s="43"/>
       <c r="S56" s="37" t="s">
         <v>33</v>
       </c>
@@ -2889,13 +3047,13 @@
       <c r="U56" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="X56" s="44" t="s">
+      <c r="X56" s="43" t="s">
         <v>39</v>
       </c>
       <c r="Y56" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="AA56" s="45" t="s">
+      <c r="AA56" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2924,20 +3082,19 @@
       <c r="B60" s="2">
         <v>45461.777777777781</v>
       </c>
-      <c r="I60" s="43"/>
       <c r="S60" s="37" t="s">
         <v>35</v>
       </c>
       <c r="T60" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="X60" s="44" t="s">
+      <c r="X60" s="43" t="s">
         <v>39</v>
       </c>
       <c r="Y60" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="AA60" s="45" t="s">
+      <c r="AA60" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2954,7 +3111,7 @@
       </c>
       <c r="S62" s="31"/>
       <c r="T62" s="31"/>
-      <c r="U62" s="44" t="s">
+      <c r="U62" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2969,17 +3126,16 @@
       <c r="B64" s="2">
         <v>45461.805555555555</v>
       </c>
-      <c r="I64" s="43"/>
       <c r="S64" s="38" t="s">
         <v>23</v>
       </c>
       <c r="T64" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="X64" s="48" t="s">
+      <c r="X64" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="Y64" s="44" t="s">
+      <c r="Y64" s="43" t="s">
         <v>39</v>
       </c>
       <c r="AA64" s="38" t="s">
@@ -2999,7 +3155,7 @@
       </c>
       <c r="S66" s="31"/>
       <c r="T66" s="31"/>
-      <c r="U66" s="44" t="s">
+      <c r="U66" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3014,7 +3170,6 @@
       <c r="B68" s="2">
         <v>45461.833333333336</v>
       </c>
-      <c r="I68" s="43"/>
       <c r="S68" s="38" t="s">
         <v>36</v>
       </c>
@@ -3041,7 +3196,7 @@
       </c>
       <c r="S70" s="31"/>
       <c r="T70" s="31"/>
-      <c r="U70" s="44" t="s">
+      <c r="U70" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3056,7 +3211,6 @@
       <c r="B72" s="2">
         <v>45461.861111111109</v>
       </c>
-      <c r="I72" s="43"/>
       <c r="S72" s="39" t="s">
         <v>34</v>
       </c>
@@ -3066,7 +3220,7 @@
       <c r="X72" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="AA72" s="43" t="s">
+      <c r="AA72" s="42" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3083,7 +3237,7 @@
       </c>
       <c r="S74" s="31"/>
       <c r="T74" s="31"/>
-      <c r="U74" s="44" t="s">
+      <c r="U74" s="43" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3098,14 +3252,13 @@
       <c r="B76" s="2">
         <v>45461.888888888891</v>
       </c>
-      <c r="I76" s="43"/>
       <c r="S76" s="40" t="s">
         <v>34</v>
       </c>
       <c r="T76" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="X76" s="49" t="s">
+      <c r="X76" s="47" t="s">
         <v>44</v>
       </c>
       <c r="AA76" s="38" t="s">
@@ -3125,7 +3278,7 @@
       </c>
       <c r="S78" s="31"/>
       <c r="T78" s="31"/>
-      <c r="U78" s="45" t="s">
+      <c r="U78" s="44" t="s">
         <v>39</v>
       </c>
     </row>
@@ -3140,14 +3293,13 @@
       <c r="B80" s="2">
         <v>45461.916666666664</v>
       </c>
-      <c r="I80" s="38"/>
       <c r="S80" s="40" t="s">
         <v>34</v>
       </c>
       <c r="T80" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="X80" s="44" t="s">
+      <c r="X80" s="43" t="s">
         <v>39</v>
       </c>
       <c r="AA80" s="38" t="s">
@@ -3182,14 +3334,13 @@
       <c r="B84" s="2">
         <v>45461.944444444445</v>
       </c>
-      <c r="I84" s="38"/>
       <c r="S84" s="40" t="s">
         <v>34</v>
       </c>
       <c r="T84" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="X84" s="44" t="s">
+      <c r="X84" s="43" t="s">
         <v>39</v>
       </c>
       <c r="AA84" s="38" t="s">
@@ -3213,25 +3364,24 @@
         <v>23</v>
       </c>
     </row>
-    <row r="87" spans="2:39" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:39" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B87" s="2">
         <v>45461.965277777781</v>
       </c>
       <c r="S87" s="33"/>
       <c r="T87" s="31"/>
     </row>
-    <row r="88" spans="2:39" ht="24.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:39" ht="18" x14ac:dyDescent="0.3">
       <c r="B88" s="2">
         <v>45461.972222222219</v>
       </c>
-      <c r="I88" s="53"/>
       <c r="S88" s="33"/>
       <c r="T88" s="31"/>
       <c r="X88" s="32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="89" spans="2:39" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:39" x14ac:dyDescent="0.3">
       <c r="B89" s="2">
         <v>45461.979166666664</v>
       </c>
@@ -3258,7 +3408,7 @@
       </c>
       <c r="S92" s="33"/>
       <c r="T92" s="31"/>
-      <c r="X92" s="43" t="s">
+      <c r="X92" s="42" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3320,25 +3470,25 @@
       <c r="T93" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="U93" s="42" t="s">
+      <c r="U93" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="V93" s="50">
+      <c r="V93" s="48">
         <v>45828</v>
       </c>
-      <c r="W93" s="50">
+      <c r="W93" s="48">
         <v>46194</v>
       </c>
-      <c r="X93" s="47" t="s">
+      <c r="X93" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="Y93" s="60" t="s">
+      <c r="Y93" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="Z93" s="79">
+      <c r="Z93" s="75">
         <v>45832</v>
       </c>
-      <c r="AA93" s="75" t="s">
+      <c r="AA93" s="71" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3346,69 +3496,69 @@
       <c r="B94" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C94" s="64"/>
-      <c r="D94" s="64"/>
-      <c r="E94" s="64"/>
-      <c r="F94" s="64"/>
-      <c r="G94" s="64"/>
-      <c r="H94" s="64"/>
-      <c r="I94" s="65"/>
-      <c r="J94" s="64"/>
-      <c r="K94" s="64"/>
-      <c r="L94" s="64"/>
-      <c r="M94" s="64"/>
-      <c r="N94" s="64"/>
-      <c r="O94" s="64"/>
-      <c r="P94" s="64"/>
-      <c r="Q94" s="64"/>
-      <c r="R94" s="64"/>
-      <c r="S94" s="65">
+      <c r="C94" s="60"/>
+      <c r="D94" s="60"/>
+      <c r="E94" s="60"/>
+      <c r="F94" s="60"/>
+      <c r="G94" s="60"/>
+      <c r="H94" s="60"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="60"/>
+      <c r="K94" s="60"/>
+      <c r="L94" s="60"/>
+      <c r="M94" s="60"/>
+      <c r="N94" s="60"/>
+      <c r="O94" s="60"/>
+      <c r="P94" s="60"/>
+      <c r="Q94" s="60"/>
+      <c r="R94" s="60"/>
+      <c r="S94" s="61">
         <v>0.41379310344827586</v>
       </c>
-      <c r="T94" s="65">
+      <c r="T94" s="61">
         <v>0.41379310344827586</v>
       </c>
-      <c r="U94" s="65">
+      <c r="U94" s="61">
         <v>0.76595744680851063</v>
       </c>
-      <c r="V94" s="66"/>
-      <c r="W94" s="67"/>
-      <c r="X94" s="65">
+      <c r="V94" s="62"/>
+      <c r="W94" s="63"/>
+      <c r="X94" s="61">
         <v>0.68932038834951459</v>
       </c>
-      <c r="Y94" s="71">
+      <c r="Y94" s="67">
         <v>0.38333333333333336</v>
       </c>
-      <c r="Z94" s="64"/>
-      <c r="AA94" s="71">
+      <c r="Z94" s="60"/>
+      <c r="AA94" s="67">
         <v>0.8666666666666667</v>
       </c>
-      <c r="AB94" s="64"/>
-      <c r="AC94" s="81"/>
-      <c r="AD94" s="64"/>
-      <c r="AE94" s="64"/>
-      <c r="AF94" s="64"/>
+      <c r="AB94" s="60"/>
+      <c r="AC94" s="80"/>
+      <c r="AD94" s="60"/>
+      <c r="AE94" s="60"/>
+      <c r="AF94" s="60"/>
     </row>
     <row r="95" spans="2:39" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B95" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C95" s="76"/>
-      <c r="D95" s="68"/>
-      <c r="E95" s="68"/>
-      <c r="F95" s="68"/>
-      <c r="G95" s="68"/>
-      <c r="H95" s="68"/>
-      <c r="I95" s="69"/>
-      <c r="J95" s="69"/>
-      <c r="K95" s="70"/>
-      <c r="L95" s="69"/>
-      <c r="M95" s="69"/>
-      <c r="N95" s="69"/>
-      <c r="O95" s="69"/>
-      <c r="P95" s="69"/>
-      <c r="Q95" s="69"/>
-      <c r="R95" s="69"/>
+      <c r="C95" s="72"/>
+      <c r="D95" s="64"/>
+      <c r="E95" s="64"/>
+      <c r="F95" s="64"/>
+      <c r="G95" s="64"/>
+      <c r="H95" s="64"/>
+      <c r="I95" s="65"/>
+      <c r="J95" s="65"/>
+      <c r="K95" s="66"/>
+      <c r="L95" s="65"/>
+      <c r="M95" s="65"/>
+      <c r="N95" s="65"/>
+      <c r="O95" s="65"/>
+      <c r="P95" s="65"/>
+      <c r="Q95" s="65"/>
+      <c r="R95" s="65"/>
       <c r="S95" s="99">
         <v>0.76595744680851097</v>
       </c>
@@ -3420,25 +3570,25 @@
       <c r="Y95" s="101">
         <v>0.38333333333333303</v>
       </c>
-      <c r="Z95" s="103">
+      <c r="Z95" s="102">
         <v>0.86666666666666703</v>
       </c>
-      <c r="AA95" s="103"/>
-      <c r="AB95" s="103"/>
-      <c r="AC95" s="103"/>
-      <c r="AD95" s="104"/>
-      <c r="AE95" s="104"/>
-      <c r="AF95" s="69"/>
-      <c r="AG95" s="63"/>
-      <c r="AH95" s="54"/>
-      <c r="AI95" s="54"/>
-      <c r="AJ95" s="54"/>
-      <c r="AK95" s="54"/>
-      <c r="AL95" s="54"/>
-      <c r="AM95" s="54"/>
+      <c r="AA95" s="102"/>
+      <c r="AB95" s="102"/>
+      <c r="AC95" s="102"/>
+      <c r="AD95" s="103"/>
+      <c r="AE95" s="103"/>
+      <c r="AF95" s="65"/>
+      <c r="AG95" s="59"/>
+      <c r="AH95" s="51"/>
+      <c r="AI95" s="51"/>
+      <c r="AJ95" s="51"/>
+      <c r="AK95" s="51"/>
+      <c r="AL95" s="51"/>
+      <c r="AM95" s="51"/>
     </row>
     <row r="96" spans="2:39" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B96" s="78" t="s">
+      <c r="B96" s="74" t="s">
         <v>11</v>
       </c>
       <c r="C96" s="84">
@@ -3473,7 +3623,7 @@
       <c r="AD96" s="86"/>
       <c r="AE96" s="86"/>
       <c r="AF96" s="87"/>
-      <c r="AG96" s="64"/>
+      <c r="AG96" s="60"/>
     </row>
     <row r="97" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B97" s="16" t="s">
@@ -3490,8 +3640,8 @@
       <c r="B99" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="J99" s="51"/>
-      <c r="K99" s="55"/>
+      <c r="J99" s="49"/>
+      <c r="K99" s="52"/>
       <c r="R99" s="35"/>
       <c r="S99" s="30">
         <v>58</v>
@@ -3502,32 +3652,32 @@
       <c r="U99" s="35">
         <v>206</v>
       </c>
-      <c r="V99" s="61">
+      <c r="V99" s="57">
         <v>0</v>
       </c>
       <c r="W99" s="35">
         <v>96</v>
       </c>
-      <c r="X99" s="57">
+      <c r="X99" s="54">
         <v>206</v>
       </c>
       <c r="Y99" s="35">
         <v>120</v>
       </c>
-      <c r="Z99" s="77">
+      <c r="Z99" s="73">
         <v>0</v>
       </c>
       <c r="AA99" s="35">
         <v>90</v>
       </c>
-      <c r="AC99" s="81"/>
+      <c r="AC99" s="80"/>
     </row>
     <row r="100" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B100" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="J100" s="51"/>
-      <c r="K100" s="55"/>
+      <c r="J100" s="49"/>
+      <c r="K100" s="52"/>
       <c r="Q100" s="30"/>
       <c r="R100" s="30"/>
       <c r="S100" s="30">
@@ -3539,51 +3689,55 @@
       <c r="U100" s="35">
         <v>128</v>
       </c>
-      <c r="V100" s="62">
+      <c r="V100" s="58">
         <v>0</v>
       </c>
       <c r="W100" s="35">
         <v>2</v>
       </c>
-      <c r="X100" s="57">
+      <c r="X100" s="54">
         <v>142</v>
       </c>
       <c r="Y100" s="35">
         <v>46</v>
       </c>
-      <c r="Z100" s="77">
+      <c r="Z100" s="73">
         <v>0</v>
       </c>
       <c r="AA100" s="35">
         <v>78</v>
       </c>
-      <c r="AC100" s="81"/>
-    </row>
-    <row r="101" spans="1:32" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AC100" s="80"/>
+    </row>
+    <row r="101" spans="1:32" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A101" s="96" t="s">
         <v>16</v>
       </c>
       <c r="B101" s="97"/>
+      <c r="C101" s="82">
+        <v>444</v>
+      </c>
+      <c r="D101" s="78"/>
     </row>
     <row r="102" spans="1:32" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="98" t="s">
         <v>17</v>
       </c>
       <c r="B102" s="97"/>
-      <c r="C102" s="72">
+      <c r="C102" s="68">
         <v>0.67198581560283699</v>
       </c>
-      <c r="D102" s="72"/>
+      <c r="D102" s="68"/>
     </row>
     <row r="103" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="B103" s="80" t="s">
+      <c r="B103" s="76" t="s">
         <v>48</v>
       </c>
-      <c r="C103" s="80">
+      <c r="C103" s="79">
         <v>6</v>
       </c>
-      <c r="D103" s="80"/>
-      <c r="E103" s="80"/>
+      <c r="D103" s="79"/>
+      <c r="E103" s="76"/>
     </row>
     <row r="104" spans="1:32" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="98" t="s">
@@ -3647,25 +3801,25 @@
       <c r="T107" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="U107" s="42" t="s">
+      <c r="U107" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="V107" s="50">
+      <c r="V107" s="48">
         <v>45828</v>
       </c>
-      <c r="W107" s="50">
+      <c r="W107" s="48">
         <v>46194</v>
       </c>
-      <c r="X107" s="47" t="s">
+      <c r="X107" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="Y107" s="60" t="s">
+      <c r="Y107" s="56" t="s">
         <v>46</v>
       </c>
-      <c r="Z107" s="79">
+      <c r="Z107" s="75">
         <v>45832</v>
       </c>
-      <c r="AA107" s="75" t="s">
+      <c r="AA107" s="71" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3673,30 +3827,30 @@
       <c r="B108" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C108" s="83"/>
-      <c r="J108" s="52"/>
-      <c r="K108" s="56"/>
+      <c r="C108" s="77"/>
+      <c r="J108" s="50"/>
+      <c r="K108" s="53"/>
+      <c r="M108" s="36">
+        <v>440</v>
+      </c>
       <c r="N108" s="36">
-        <v>440</v>
+        <v>480</v>
       </c>
       <c r="O108" s="36">
-        <v>480</v>
-      </c>
-      <c r="P108" s="36">
         <f>(2+4+10+10+10+10+10+8+8)*20</f>
         <v>1440</v>
       </c>
+      <c r="P108" s="36">
+        <v>0</v>
+      </c>
       <c r="Q108" s="36">
         <v>0</v>
       </c>
       <c r="R108" s="36">
-        <v>0</v>
-      </c>
-      <c r="S108" s="36">
         <v>2896</v>
       </c>
       <c r="T108" s="36"/>
-      <c r="X108" s="58">
+      <c r="X108" s="55">
         <v>3218</v>
       </c>
       <c r="Y108" s="36">
@@ -3705,81 +3859,88 @@
       <c r="AA108" s="36">
         <v>1560</v>
       </c>
-      <c r="AC108" s="82"/>
-    </row>
-    <row r="109" spans="1:32" ht="23.4" x14ac:dyDescent="0.3">
-      <c r="M109" s="88">
-        <v>5256</v>
-      </c>
-      <c r="N109" s="89"/>
-      <c r="O109" s="89"/>
-      <c r="P109" s="90"/>
-      <c r="Q109" s="89"/>
-      <c r="R109" s="89"/>
-      <c r="S109" s="91"/>
+      <c r="AC108" s="81"/>
+    </row>
+    <row r="109" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="Z109" s="104"/>
+      <c r="AA109" s="104"/>
+      <c r="AB109" s="104"/>
+      <c r="AC109" s="104"/>
+      <c r="AD109" s="104"/>
+      <c r="AE109" s="104"/>
+      <c r="AF109" s="104"/>
     </row>
     <row r="110" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B110" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="J110" s="51"/>
-      <c r="K110" s="55"/>
-      <c r="S110" s="102">
+      <c r="J110" s="49"/>
+      <c r="L110" s="88">
+        <v>5256</v>
+      </c>
+      <c r="M110" s="89"/>
+      <c r="N110" s="89"/>
+      <c r="O110" s="90"/>
+      <c r="P110" s="89"/>
+      <c r="Q110" s="89"/>
+      <c r="R110" s="91"/>
+      <c r="S110" s="83">
         <v>4276</v>
       </c>
-      <c r="T110" s="102"/>
-      <c r="U110" s="102"/>
-      <c r="V110" s="102"/>
-      <c r="W110" s="102"/>
-      <c r="X110" s="102"/>
-      <c r="Y110" s="102">
+      <c r="T110" s="83"/>
+      <c r="U110" s="83"/>
+      <c r="V110" s="83"/>
+      <c r="W110" s="83"/>
+      <c r="X110" s="83"/>
+      <c r="Y110" s="83">
         <v>1058</v>
       </c>
-      <c r="Z110" s="102">
+      <c r="Z110" s="83">
         <v>1560</v>
       </c>
-      <c r="AA110" s="97"/>
-      <c r="AB110" s="97"/>
-      <c r="AC110" s="97"/>
-      <c r="AD110" s="97"/>
-      <c r="AE110" s="97"/>
+      <c r="AA110" s="83"/>
+      <c r="AB110" s="83"/>
+      <c r="AC110" s="83"/>
+      <c r="AD110" s="83"/>
+      <c r="AE110" s="83"/>
+      <c r="AF110" s="83"/>
     </row>
     <row r="112" spans="1:32" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B112" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C112" s="102">
+      <c r="C112" s="83">
         <v>11092</v>
       </c>
-      <c r="D112" s="102"/>
-      <c r="E112" s="102"/>
-      <c r="F112" s="102"/>
-      <c r="G112" s="102"/>
-      <c r="H112" s="102"/>
-      <c r="I112" s="102"/>
-      <c r="J112" s="102"/>
-      <c r="K112" s="102"/>
-      <c r="L112" s="102"/>
-      <c r="M112" s="102"/>
-      <c r="N112" s="102"/>
-      <c r="O112" s="102"/>
-      <c r="P112" s="102"/>
-      <c r="Q112" s="102"/>
-      <c r="R112" s="102"/>
-      <c r="S112" s="102"/>
-      <c r="T112" s="102"/>
-      <c r="U112" s="102"/>
-      <c r="V112" s="102"/>
-      <c r="W112" s="102"/>
-      <c r="X112" s="102"/>
-      <c r="Y112" s="102"/>
-      <c r="Z112" s="102"/>
-      <c r="AA112" s="102"/>
-      <c r="AB112" s="102"/>
-      <c r="AC112" s="102"/>
-      <c r="AD112" s="102"/>
-      <c r="AE112" s="102"/>
-      <c r="AF112" s="102"/>
+      <c r="D112" s="83"/>
+      <c r="E112" s="83"/>
+      <c r="F112" s="83"/>
+      <c r="G112" s="83"/>
+      <c r="H112" s="83"/>
+      <c r="I112" s="83"/>
+      <c r="J112" s="83"/>
+      <c r="K112" s="83"/>
+      <c r="L112" s="83"/>
+      <c r="M112" s="83"/>
+      <c r="N112" s="83"/>
+      <c r="O112" s="83"/>
+      <c r="P112" s="83"/>
+      <c r="Q112" s="83"/>
+      <c r="R112" s="83"/>
+      <c r="S112" s="83"/>
+      <c r="T112" s="83"/>
+      <c r="U112" s="83"/>
+      <c r="V112" s="83"/>
+      <c r="W112" s="83"/>
+      <c r="X112" s="83"/>
+      <c r="Y112" s="83"/>
+      <c r="Z112" s="83"/>
+      <c r="AA112" s="83"/>
+      <c r="AB112" s="83"/>
+      <c r="AC112" s="83"/>
+      <c r="AD112" s="83"/>
+      <c r="AE112" s="83"/>
+      <c r="AF112" s="83"/>
     </row>
     <row r="114" spans="2:2" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B114" s="20" t="s">
@@ -3830,7 +3991,7 @@
   <mergeCells count="11">
     <mergeCell ref="C112:AF112"/>
     <mergeCell ref="C96:AF96"/>
-    <mergeCell ref="M109:S109"/>
+    <mergeCell ref="L110:R110"/>
     <mergeCell ref="C4:D5"/>
     <mergeCell ref="A101:B101"/>
     <mergeCell ref="A102:B102"/>
@@ -3838,7 +3999,7 @@
     <mergeCell ref="S95:Y95"/>
     <mergeCell ref="S110:Y110"/>
     <mergeCell ref="Z95:AE95"/>
-    <mergeCell ref="Z110:AE110"/>
+    <mergeCell ref="Z110:AF110"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>